<commit_message>
Updated docs and have a new result
</commit_message>
<xml_diff>
--- a/SummerWork/TEST_OUTPUT.xlsx
+++ b/SummerWork/TEST_OUTPUT.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="275">
   <si>
     <t>School Name :</t>
   </si>
@@ -422,6 +422,423 @@
   </si>
   <si>
     <t xml:space="preserve">Besides volunteer resources (medical and field study instruction) no other funding resources were pursued. </t>
+  </si>
+  <si>
+    <t>Please describe how your program serves historically underrepresented populations. What actions are you taking to make this an experience for all students to thrive? (Select and briefly describe all that apply.)</t>
+  </si>
+  <si>
+    <t>Other: medical issues</t>
+  </si>
+  <si>
+    <t>Amity Elementary School</t>
+  </si>
+  <si>
+    <t>Amity SD 4J</t>
+  </si>
+  <si>
+    <t>Diana Sohn</t>
+  </si>
+  <si>
+    <t>diana.sohn@amity.k12.or.us</t>
+  </si>
+  <si>
+    <t>503-835-3751 ext 314</t>
+  </si>
+  <si>
+    <t>503-835-3751 ext. 314</t>
+  </si>
+  <si>
+    <t>We provide a number of hands-on inquiry based activities and experiences that are integrated with our science, technology, engineering, and mathematics curricula.  For example:  building shelters, determining calories, fishing,…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We have at least 1 high school counselor who helps with translations during ODS meetings for parents and is with the ELL student during camp to help with understanding of the content/concepts. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Students and families are not charged money to participate. Fundraising has been done by the students to keep this program running for over 35 years.   All 5th grade children attend and have done so for over 35 years.  No one is excluded based on socio-economic status.  Many of our experiences take place in areas that our students have not had the opportunity to visit. </t>
+  </si>
+  <si>
+    <t>Amity is a rural community, during Outdoor School, we visit a variety of terrain (forest, desert, cave, National Park, State Park, museums, nature centers) to show the differences and similarities throughout Oregon and how we depend on each other.</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Student journals are used when we get back to reflect upon our experiences. Journals are also used to interact with other students about what they learned. Pre- ODS we visited the Evergreen Museum and Cruickshank Farms to gain some pre knowledge about space and timber topics. Post- writing thank you letters to counselors, parents, bus drivers, and teachers. Students also wrote an ODS memory reflecting on their favorite activity from camp. Our science curriculum revolves around our Outdoor School and is integrated throughout the year.</t>
+  </si>
+  <si>
+    <t>The chaperones are high school students grades 10-12th with good grades and approval of their teachers. High School students are responsible for a small tent group and teaching a study session six times.  They are on duty 23 hours a day for four days.  They also receive 20 hours of training prior to Outdoor School.  This past year over 40 parents/grandparents attended and helped with kitchen duties, recreation, and setup and break down of camp. One of the bus drivers is the chief of the fire department in town, who volunteers his time.  We also have at least four community members who volunteer to help with cooking.</t>
+  </si>
+  <si>
+    <t>In science, 68% of students passed the OAKS Science test due to their experiences at ODS. Without these experiences students would not have done as well.  Students have learned how to properly write thank you notes and reflections.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Many students volunteered hours upon hours to help prepare for ODS. It empowered students to become leaders in their community and in the classroom. Students that volunteered were able to submit hours for their Presidential Volunteer Pin. The high school counselors received over 100 hours of volunteer hours-which displays their leadership skills in running study sessions and leading their groups. </t>
+  </si>
+  <si>
+    <t>Because students know they have to be respectful, responsible, and safe to attend Outdoor School, classroom management and discipline problems are minimal.  Students who have behavior or missing work issues are placed on Outdoor School contracts and the majority of these students improve their behaviors.</t>
+  </si>
+  <si>
+    <t>Students earn beads and awards in camp that transfer back to the classroom when we return.  It builds community within their class.</t>
+  </si>
+  <si>
+    <t>Outdoor School provides students the opportunity to improve their problem solving and strategic thinking due to the open ended experiences.  For example, in survival - how to build a shelter, how to fix their leaking tent, how to take care of personal needs independently, and how to think fast when it came to a thunder and lightning storm.</t>
+  </si>
+  <si>
+    <t>Students had opportunities to create shelters, make and present songs and skits, weave a design on a loom, build a nutritious parfait, create an obstacle course.</t>
+  </si>
+  <si>
+    <t>Students were in a variety of groups during study sessions, tent groups, field trips away from camps, recreation, and partner work where they had to communicate with their peers in order to successfully complete tasks.</t>
+  </si>
+  <si>
+    <t>Our students were very enthusiastic about science (space, birds, volcanic activity, animals) and social studies (High Desert Museum).  Looking through telescopes, observing animals, exploring caves resulted in excitement about learning new things.</t>
+  </si>
+  <si>
+    <t>The Sun River Nature Center experience increased our students' understanding of birds of prey, desert habitat, interdependence of living things, animal adaptations, and space.  Fishing, nutrition, survival, and nature study sessions also helped students better understand science.</t>
+  </si>
+  <si>
+    <t>During our Woodland Tour, students learn the importance of fire prevention, the impact of fires, the effect of litter on land and streams, soil erosion impact, laws and rules in the wilderness, and how to be a better environmental citizen.</t>
+  </si>
+  <si>
+    <t>Before we leave, students  research and calculate the cost of Outdoor School including gas, meals, entrance fees, and camping fees.  They determine the total and cost per student.</t>
+  </si>
+  <si>
+    <t>Students articulate through songs and skits.  They also complete a Outdoor School journal and reflection that requires reading, writing, listening, and speaking skills.</t>
+  </si>
+  <si>
+    <t>Students improve their social studies understanding through historical information and exhibits at the museum, nature center, and visitor centers.  Students learn about Native American culture, history, and crafts.</t>
+  </si>
+  <si>
+    <t>All students, regardless of abilities, medical conditions, or socio-economic status can attend Outdoor School at no cost.  We work hard to meet these individual needs.</t>
+  </si>
+  <si>
+    <t>For our limited English student, we provided a counselor who spoke Spanish and assisted the student.  Curriculum is translated as much as possible.</t>
+  </si>
+  <si>
+    <t>Special education students receive assistance from their counselors.  Accommodations are provided to help them be successful. 1:1 if necessary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Learning disabled students receive assistance from their counselors.  Accommodations are provided to help them be successful.  </t>
+  </si>
+  <si>
+    <t>Items needed are purchased for the student.  Counselor helps with any needs.</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>Translator and translations when needed.  Spanish speaking counselor.</t>
+  </si>
+  <si>
+    <t>Accommodations so they can fully participate.  (diabetes, asthma, epilepsy)</t>
+  </si>
+  <si>
+    <t>At Amity Elementary School, all students are offered the opportunity to participate in Outdoor School.  Historically, we have only left behind students who are a danger to themselves or others and those with excessive missing work (even after numerous options and opportunities are given).  98% of 5th graders attend.</t>
+  </si>
+  <si>
+    <t>Local fundraisers:  Stuff the Envelope, Community-School Dinners, Box-Tops, Jog-a-Thon, and Wreath Sales</t>
+  </si>
+  <si>
+    <t>Arlington School District #3</t>
+  </si>
+  <si>
+    <t>Arlington SD 3</t>
+  </si>
+  <si>
+    <t>Kevin Hunking</t>
+  </si>
+  <si>
+    <t>khunking@arlington.k12.or.us</t>
+  </si>
+  <si>
+    <t>541-454-2632</t>
+  </si>
+  <si>
+    <t>Follows core standards and integrates science, engineering, and math. Students learned orienteering and map reading.</t>
+  </si>
+  <si>
+    <t>Teachers speak english and spanish.</t>
+  </si>
+  <si>
+    <t>All students had equal access.</t>
+  </si>
+  <si>
+    <t>Students learn about their communities and local environment.</t>
+  </si>
+  <si>
+    <t>Classroom discussion about outdoor school activities.</t>
+  </si>
+  <si>
+    <t>Parents provided feedback and rangers helped teach classes.</t>
+  </si>
+  <si>
+    <t>Students received awards for completing achievements.</t>
+  </si>
+  <si>
+    <t>Learned problem solving strategies as a group.</t>
+  </si>
+  <si>
+    <t>Learned to communicate with leaders and other students.</t>
+  </si>
+  <si>
+    <t>Learned orienteering and map reading.</t>
+  </si>
+  <si>
+    <t>Learned to read maps.</t>
+  </si>
+  <si>
+    <t>Map reading.</t>
+  </si>
+  <si>
+    <t>Reading and communication skills.</t>
+  </si>
+  <si>
+    <t>Learned about our community and history.</t>
+  </si>
+  <si>
+    <t>All students received differentiated instruction.</t>
+  </si>
+  <si>
+    <t>Our students all live in a rural community.</t>
+  </si>
+  <si>
+    <t>Instruction was available in other languages.</t>
+  </si>
+  <si>
+    <t>Support staff was involved with special education students.</t>
+  </si>
+  <si>
+    <t>All students received the same instruction.</t>
+  </si>
+  <si>
+    <t>All students in grade 6 attend outdoor school as part of the curriculum.</t>
+  </si>
+  <si>
+    <t>Park Rangers donated instructional time.</t>
+  </si>
+  <si>
+    <t>AMS</t>
+  </si>
+  <si>
+    <t>Ashland SD 5</t>
+  </si>
+  <si>
+    <t>Hillary Harper</t>
+  </si>
+  <si>
+    <t>Alana Valencia</t>
+  </si>
+  <si>
+    <t>hillary.harper@ashland.k12.or.us</t>
+  </si>
+  <si>
+    <t>alana.valencia@ashland.k12.or.us</t>
+  </si>
+  <si>
+    <t>541-482-1611</t>
+  </si>
+  <si>
+    <t>541-481-2811</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All lessons are alligned to Oregon State Standarsds and NGSS. </t>
+  </si>
+  <si>
+    <t>Forms are produced in Spanish when necessary.</t>
+  </si>
+  <si>
+    <t>All students are allowed to participate regardless of financial ability, scholarships and equipment are provided.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pre and post assesments are given, comprehensive ecology unit is taught around the experience. Some teachers have received outdoor ed professional development regarding outdoor ed.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">We have partnered with both the local high school to provide counselors and with the local university to provide instructors. Parents are encouraged to attend as volunteers counselors. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">students come back from ROS with greater self sufficiency and leadership skills. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">increase in student engagement, students reflect fondly on the experience as they move through the middle school. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">we are able to work with student on positive problem solving skills which can be brought back into the classroom. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">students are able to creatively think about the interconnectedness of nature. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">living in a cabin with 8 other students over the course of the trip allows ample time to practice communication skills and ability to work. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Students come back to school excited about their experience and this is carried through to all subject areas. </t>
+  </si>
+  <si>
+    <t>NGSS and Oregon State Science Standards are taught.</t>
+  </si>
+  <si>
+    <t>field studies allow students to practice real world science.</t>
+  </si>
+  <si>
+    <t>some math  (measurement, angles, compass work, ) is practiced.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">some writing and creative arts are used in field studies as well as presentation of findings. </t>
+  </si>
+  <si>
+    <t>maps are used, and ways humans impact the environment are investigated.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">multiple intelligences and learning styles are addressed in field stations and the experience is available to all students regardless of ability. </t>
+  </si>
+  <si>
+    <t>spanish forms are available</t>
+  </si>
+  <si>
+    <t>EA support, 1 on 1 staffing, provided as necessary so all students can attend</t>
+  </si>
+  <si>
+    <t>all students are allowed to attend regardless of financial ability, scholarships are available as well as equipment</t>
+  </si>
+  <si>
+    <t>all students are allowed to attend regardless of financial ability, scholarships are available as well as equipment.EA support, 1 on 1 staffing, provided as necessary so all students can attend</t>
+  </si>
+  <si>
+    <t>parent funding, district funding</t>
+  </si>
+  <si>
+    <t>Willow Wind</t>
+  </si>
+  <si>
+    <t>Ashland</t>
+  </si>
+  <si>
+    <t>Linda Terry</t>
+  </si>
+  <si>
+    <t>Linda.Terry@ashland.k12.or.us</t>
+  </si>
+  <si>
+    <t>541-488-2684</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OMSI Outdoor Science School (the ODS used this year) provides a concept-based environmental program whereby activities are closely aligned with (and therefore are integrated with) Next Generation Science Standards, which have been implemented at Willow Wind.  This program takes place at Hancock Field Station, which is located on site at John Day Fossil Beds National Monument in Central Oregon.  Field studies include a day-long study of the geology/paleontology of John Day formations, and short-term courses will include avian studies, arid lands ecology, and orienteering, with evening programs in observational astronomy and the crepuscular habits of desert animals.  </t>
+  </si>
+  <si>
+    <t>Several instructional leaders at OMSI Hancock Field Station are bilingual, so this option is presumably available if needed.</t>
+  </si>
+  <si>
+    <t>Funding that covers the cost for all students to participate in ODS is the key to ensuring equity.  Without this support, many students would not be able to participate and reap the substantial benefits that ODS provides.</t>
+  </si>
+  <si>
+    <t>Discussions between OMSI faciliators and students focused primarily on how urban areas were dependent on rural areas, with an emphasis on water use, food production and wildlands management.</t>
+  </si>
+  <si>
+    <t>Pre-activities consisted primarily of learning about John Day Fossil Beds and how students should prepare for their experience in a new environment.  Post-activites included extended studies of ecosystems dynamics, energy transfer in ecosystems and geologic processes/paleontology/geologic history.</t>
+  </si>
+  <si>
+    <t>Parent volunteers assisted with organizing the ODS, and also volunteered as chaperones.</t>
+  </si>
+  <si>
+    <t>Successful to some degree, although this is difficult to measure.</t>
+  </si>
+  <si>
+    <t>Significant growth was noted among many students, particularly those who had not participated in overnight activites without parents.  Students learned that they could make decisions without input from parents, which built confidence.</t>
+  </si>
+  <si>
+    <t>Some students really blossomed in this environment-they were held to a high behavior expectation, and almost uniformly rose to the occasion.</t>
+  </si>
+  <si>
+    <t>Successful, especially since students were expected to help with meal prep and cleanup; it was clear that for some students, this type of responsibility was new.</t>
+  </si>
+  <si>
+    <t>Highly successful</t>
+  </si>
+  <si>
+    <t>Greater enthusiasm for science</t>
+  </si>
+  <si>
+    <t>n/a (minimal)</t>
+  </si>
+  <si>
+    <t>Somewhat successful</t>
+  </si>
+  <si>
+    <t>Trip equipment and supplies were provided to students who required this support.</t>
+  </si>
+  <si>
+    <t>Support will continue to be provided so that all students at Willow Wind can participate in ODS.</t>
+  </si>
+  <si>
+    <t>Ashland School District covered any costs not covered through grant monies.  Supplies for students were provided by parents and school staff.</t>
+  </si>
+  <si>
+    <t>John Muir</t>
+  </si>
+  <si>
+    <t>James Bowers   Marcia Ososke</t>
+  </si>
+  <si>
+    <t>James.Bowers@Ashland.k12.or.us    Marcia.Ososke@Ashland.k12.or.us</t>
+  </si>
+  <si>
+    <t>541-482-8577</t>
+  </si>
+  <si>
+    <t>Next Generation Science Standards:  MS-LS2-4;  MS-LS2-5;  MS-LS4-2; MS-ESS2-4; MS-ESS3-3;  MS-Ess3-4;  MS-ESS3-5</t>
+  </si>
+  <si>
+    <t>Not offered bilingually.</t>
+  </si>
+  <si>
+    <t>We provided students with the opportunity to study "Ecosystems" that were distant from our region.  In traveling to the Oregon Coast, we studied the differences in ecosystems in regards to forests, water, ocean and estuaries.  Students learned not only about "what makes an ecosystem," but about current events that effect the health of ecosystems from the coast to the Rogue Valley.  Students visited the coast, hiking along part of the Oregon Coast Trail, visiting Shore Acres State Park, Cape Arago, Sunset Bay State Park and South Slough National Marine Estuary.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">See attached.  Students worked with focus questions looking at how rural economies are dependent upon the natural environment.  We invited biologists from Oregon Department of Fish and Wildlife to discuss work on rural watersheds to manage for habitat while sustaining the local environment.  At South Slough Estuary, students learned about local costal watersheds and the factors that impact them in regards to maintaining biodiversity.  </t>
+  </si>
+  <si>
+    <t>Hands-on experiences through hiking, observing, journaling and discussing.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Students completed experiential education reflections regarding their involvement in the trip, along with observations and big-picture learnings.  </t>
+  </si>
+  <si>
+    <t>Parents joined on this trip to assist as chaperones in yurts and tents and to help with managing students, along with preparing meals.  We worked with Sunset Bay State Park rangers to do a service learning project, removing blackberries around the park, as a means of aquiring a discount on rental rates.  We also made the connection between managing invasive species in an ecosystem.  We coordinated with educators at South Slough National Marine Estuary in guided hikes to learn about the importance of the estuary ecosystem in the region.  Rangers from the Oregon Department of Fish and Wildlife met with our group one evening to teach about ecosystem management, we did a tour of the Washed Ashore museum in Bandon to learn about human impacts on the ocean environment on our last day.  Also, on the third day we met with an educator from Costal Ecosystem Partners in Education to learn about bird migration and habitat protection.  On our first night, we took students to visit Siuslaw Tribal Elders in Coos Bay to learn about Native Peoples' relationship to the land and the transition of land ownership in the area.  Students learned native ways of agriculture, hunting and ceremonial traditions.</t>
+  </si>
+  <si>
+    <t>As a school we score well on district assessments (Easy CBM) and state/national assessements (Smarter Balanced)</t>
+  </si>
+  <si>
+    <t>Doing a fall over night trip in particular helps build leadership skills right from the start of the school year.  Every year we see students brave the elements and become more confident people.</t>
+  </si>
+  <si>
+    <t>We see classmates bond and not want to let each other down this leads to fewer discipline and management problems.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I think so but no data (quantitive or quailitative) around this.  If there was a survey of something for the students to fill out after the trip it may give us this type of information. </t>
+  </si>
+  <si>
+    <t>Outdoor expereinces all allow for all students to thrive.  This especially goes for students who may struggle more through tradtional acedemic classroom expereinces.</t>
+  </si>
+  <si>
+    <t>Visuals and hands-on experiences.  Lots of opportunities to work in groups.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Educational assistants joined on trip to assist with learnings.  Activities were modified for students in terms of pace and directions.  </t>
+  </si>
+  <si>
+    <t>No major disabilities with students - lots of parent support and staff support for those who might have struggled either emotionally or socially.</t>
+  </si>
+  <si>
+    <t>Gear provided by the school for all students.  Food provided.</t>
+  </si>
+  <si>
+    <t>Connected students to Native American tribal traditions with Siuslaw Tribe in Coos Bay.</t>
+  </si>
+  <si>
+    <t>This trip is required for all students in our school.  We provide gear, food, lodging and transportation for all students, regardless of economic level.  We fundraise as part of our Parent Teacher Collective to scholarship any needs students or families may have.  It is so great to have the outdoor school funds as it takes some financial pressure off of the district and our own Parent Teacher Collective.  Curriculum in the classroom was integrated with trip studies.</t>
+  </si>
+  <si>
+    <t>Parents attended trip, using personal vehicles and donating gas costs.  Cooking equipment and gear were provided by parents.  Coordinated with Sunset Bay State Park to do community service for discounted camping rates.  District pays for fuel for busses.</t>
   </si>
 </sst>
 </file>
@@ -770,7 +1187,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BP4"/>
+  <dimension ref="A1:BP9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1399,6 +1816,937 @@
         <v>135</v>
       </c>
     </row>
+    <row r="5" spans="1:68">
+      <c r="A5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C5" t="s">
+        <v>140</v>
+      </c>
+      <c r="D5" t="s">
+        <v>140</v>
+      </c>
+      <c r="E5" t="s">
+        <v>141</v>
+      </c>
+      <c r="F5" t="s">
+        <v>141</v>
+      </c>
+      <c r="G5" t="s">
+        <v>142</v>
+      </c>
+      <c r="H5" t="s">
+        <v>143</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5">
+        <v>3</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <v>4</v>
+      </c>
+      <c r="M5">
+        <v>5</v>
+      </c>
+      <c r="N5">
+        <v>5</v>
+      </c>
+      <c r="O5">
+        <v>3</v>
+      </c>
+      <c r="P5">
+        <v>4</v>
+      </c>
+      <c r="Q5">
+        <v>4</v>
+      </c>
+      <c r="R5">
+        <v>3</v>
+      </c>
+      <c r="S5">
+        <v>3</v>
+      </c>
+      <c r="T5">
+        <v>5</v>
+      </c>
+      <c r="U5">
+        <v>4</v>
+      </c>
+      <c r="V5">
+        <v>3</v>
+      </c>
+      <c r="W5">
+        <v>5</v>
+      </c>
+      <c r="X5">
+        <v>4</v>
+      </c>
+      <c r="Y5">
+        <v>5</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>144</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>145</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>146</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>147</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>148</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>148</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>148</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>148</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>148</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>148</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>122</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>149</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>150</v>
+      </c>
+      <c r="AO5" t="s">
+        <v>151</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>152</v>
+      </c>
+      <c r="AQ5" t="s">
+        <v>153</v>
+      </c>
+      <c r="AR5" t="s">
+        <v>154</v>
+      </c>
+      <c r="AS5" t="s">
+        <v>155</v>
+      </c>
+      <c r="AT5" t="s">
+        <v>156</v>
+      </c>
+      <c r="AU5" t="s">
+        <v>157</v>
+      </c>
+      <c r="AV5" t="s">
+        <v>158</v>
+      </c>
+      <c r="AW5" t="s">
+        <v>159</v>
+      </c>
+      <c r="AX5" t="s">
+        <v>160</v>
+      </c>
+      <c r="AY5" t="s">
+        <v>161</v>
+      </c>
+      <c r="AZ5" t="s">
+        <v>162</v>
+      </c>
+      <c r="BA5" t="s">
+        <v>163</v>
+      </c>
+      <c r="BB5" t="s">
+        <v>164</v>
+      </c>
+      <c r="BD5" t="s">
+        <v>165</v>
+      </c>
+      <c r="BE5" t="s">
+        <v>166</v>
+      </c>
+      <c r="BF5" t="s">
+        <v>167</v>
+      </c>
+      <c r="BG5" t="s">
+        <v>168</v>
+      </c>
+      <c r="BH5" t="s">
+        <v>169</v>
+      </c>
+      <c r="BI5" t="s">
+        <v>169</v>
+      </c>
+      <c r="BJ5" t="s">
+        <v>169</v>
+      </c>
+      <c r="BK5" t="s">
+        <v>169</v>
+      </c>
+      <c r="BL5" t="s">
+        <v>170</v>
+      </c>
+      <c r="BM5" t="s">
+        <v>171</v>
+      </c>
+      <c r="BN5" t="s">
+        <v>172</v>
+      </c>
+      <c r="BP5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="6" spans="1:68">
+      <c r="A6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B6" t="s">
+        <v>175</v>
+      </c>
+      <c r="C6" t="s">
+        <v>176</v>
+      </c>
+      <c r="D6" t="s">
+        <v>176</v>
+      </c>
+      <c r="E6" t="s">
+        <v>177</v>
+      </c>
+      <c r="F6" t="s">
+        <v>177</v>
+      </c>
+      <c r="G6" t="s">
+        <v>178</v>
+      </c>
+      <c r="H6" t="s">
+        <v>178</v>
+      </c>
+      <c r="I6">
+        <v>4</v>
+      </c>
+      <c r="J6">
+        <v>5</v>
+      </c>
+      <c r="K6">
+        <v>5</v>
+      </c>
+      <c r="L6">
+        <v>3</v>
+      </c>
+      <c r="M6">
+        <v>4</v>
+      </c>
+      <c r="N6">
+        <v>4</v>
+      </c>
+      <c r="O6">
+        <v>2</v>
+      </c>
+      <c r="P6">
+        <v>3</v>
+      </c>
+      <c r="Q6">
+        <v>3</v>
+      </c>
+      <c r="R6">
+        <v>3</v>
+      </c>
+      <c r="S6">
+        <v>2</v>
+      </c>
+      <c r="T6">
+        <v>2</v>
+      </c>
+      <c r="U6">
+        <v>2</v>
+      </c>
+      <c r="V6">
+        <v>4</v>
+      </c>
+      <c r="W6">
+        <v>5</v>
+      </c>
+      <c r="X6">
+        <v>1</v>
+      </c>
+      <c r="Y6">
+        <v>2</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>179</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>180</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>181</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>182</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>148</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>148</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>148</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>148</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>148</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>148</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>148</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>122</v>
+      </c>
+      <c r="AM6" t="s">
+        <v>183</v>
+      </c>
+      <c r="AN6" t="s">
+        <v>184</v>
+      </c>
+      <c r="AO6" t="s">
+        <v>134</v>
+      </c>
+      <c r="AP6" t="s">
+        <v>185</v>
+      </c>
+      <c r="AQ6" t="s">
+        <v>134</v>
+      </c>
+      <c r="AR6" t="s">
+        <v>185</v>
+      </c>
+      <c r="AS6" t="s">
+        <v>186</v>
+      </c>
+      <c r="AT6" t="s">
+        <v>134</v>
+      </c>
+      <c r="AU6" t="s">
+        <v>187</v>
+      </c>
+      <c r="AV6" t="s">
+        <v>134</v>
+      </c>
+      <c r="AW6" t="s">
+        <v>188</v>
+      </c>
+      <c r="AX6" t="s">
+        <v>189</v>
+      </c>
+      <c r="AY6" t="s">
+        <v>190</v>
+      </c>
+      <c r="AZ6" t="s">
+        <v>191</v>
+      </c>
+      <c r="BA6" t="s">
+        <v>192</v>
+      </c>
+      <c r="BB6" t="s">
+        <v>193</v>
+      </c>
+      <c r="BC6" t="s">
+        <v>194</v>
+      </c>
+      <c r="BD6" t="s">
+        <v>195</v>
+      </c>
+      <c r="BE6" t="s">
+        <v>196</v>
+      </c>
+      <c r="BF6" t="s">
+        <v>196</v>
+      </c>
+      <c r="BG6" t="s">
+        <v>197</v>
+      </c>
+      <c r="BH6" t="s">
+        <v>134</v>
+      </c>
+      <c r="BI6" t="s">
+        <v>134</v>
+      </c>
+      <c r="BJ6" t="s">
+        <v>134</v>
+      </c>
+      <c r="BK6" t="s">
+        <v>134</v>
+      </c>
+      <c r="BL6" t="s">
+        <v>195</v>
+      </c>
+      <c r="BN6" t="s">
+        <v>198</v>
+      </c>
+      <c r="BO6" t="s">
+        <v>134</v>
+      </c>
+      <c r="BP6" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="7" spans="1:68">
+      <c r="A7" t="s">
+        <v>200</v>
+      </c>
+      <c r="B7" t="s">
+        <v>201</v>
+      </c>
+      <c r="C7" t="s">
+        <v>202</v>
+      </c>
+      <c r="D7" t="s">
+        <v>203</v>
+      </c>
+      <c r="E7" t="s">
+        <v>204</v>
+      </c>
+      <c r="F7" t="s">
+        <v>205</v>
+      </c>
+      <c r="G7" t="s">
+        <v>206</v>
+      </c>
+      <c r="H7" t="s">
+        <v>207</v>
+      </c>
+      <c r="I7">
+        <v>5</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>4</v>
+      </c>
+      <c r="L7">
+        <v>4</v>
+      </c>
+      <c r="M7">
+        <v>5</v>
+      </c>
+      <c r="N7">
+        <v>5</v>
+      </c>
+      <c r="O7">
+        <v>3</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>2</v>
+      </c>
+      <c r="R7">
+        <v>4</v>
+      </c>
+      <c r="S7">
+        <v>2</v>
+      </c>
+      <c r="T7">
+        <v>3</v>
+      </c>
+      <c r="U7">
+        <v>3</v>
+      </c>
+      <c r="V7">
+        <v>4</v>
+      </c>
+      <c r="W7">
+        <v>3</v>
+      </c>
+      <c r="X7">
+        <v>2</v>
+      </c>
+      <c r="Y7">
+        <v>5</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>208</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>209</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>210</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>108</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>148</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>148</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>148</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>148</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>122</v>
+      </c>
+      <c r="AM7" t="s">
+        <v>211</v>
+      </c>
+      <c r="AN7" t="s">
+        <v>212</v>
+      </c>
+      <c r="AO7" t="s">
+        <v>108</v>
+      </c>
+      <c r="AP7" t="s">
+        <v>213</v>
+      </c>
+      <c r="AQ7" t="s">
+        <v>108</v>
+      </c>
+      <c r="AR7" t="s">
+        <v>214</v>
+      </c>
+      <c r="AS7" t="s">
+        <v>215</v>
+      </c>
+      <c r="AT7" t="s">
+        <v>216</v>
+      </c>
+      <c r="AU7" t="s">
+        <v>217</v>
+      </c>
+      <c r="AV7" t="s">
+        <v>218</v>
+      </c>
+      <c r="AW7" t="s">
+        <v>219</v>
+      </c>
+      <c r="AX7" t="s">
+        <v>220</v>
+      </c>
+      <c r="AY7" t="s">
+        <v>221</v>
+      </c>
+      <c r="AZ7" t="s">
+        <v>222</v>
+      </c>
+      <c r="BA7" t="s">
+        <v>223</v>
+      </c>
+      <c r="BB7" t="s">
+        <v>224</v>
+      </c>
+      <c r="BD7" t="s">
+        <v>225</v>
+      </c>
+      <c r="BE7" t="s">
+        <v>226</v>
+      </c>
+      <c r="BG7" t="s">
+        <v>227</v>
+      </c>
+      <c r="BN7" t="s">
+        <v>228</v>
+      </c>
+      <c r="BP7" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="8" spans="1:68">
+      <c r="A8" t="s">
+        <v>230</v>
+      </c>
+      <c r="B8" t="s">
+        <v>231</v>
+      </c>
+      <c r="C8" t="s">
+        <v>232</v>
+      </c>
+      <c r="D8" t="s">
+        <v>203</v>
+      </c>
+      <c r="E8" t="s">
+        <v>233</v>
+      </c>
+      <c r="F8" t="s">
+        <v>205</v>
+      </c>
+      <c r="G8" t="s">
+        <v>234</v>
+      </c>
+      <c r="H8" t="s">
+        <v>207</v>
+      </c>
+      <c r="I8">
+        <v>5</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>3</v>
+      </c>
+      <c r="L8">
+        <v>4</v>
+      </c>
+      <c r="M8">
+        <v>5</v>
+      </c>
+      <c r="N8">
+        <v>5</v>
+      </c>
+      <c r="O8">
+        <v>3</v>
+      </c>
+      <c r="P8">
+        <v>4</v>
+      </c>
+      <c r="Q8">
+        <v>3</v>
+      </c>
+      <c r="R8">
+        <v>5</v>
+      </c>
+      <c r="S8">
+        <v>2</v>
+      </c>
+      <c r="T8">
+        <v>2</v>
+      </c>
+      <c r="U8">
+        <v>3</v>
+      </c>
+      <c r="V8">
+        <v>5</v>
+      </c>
+      <c r="W8">
+        <v>5</v>
+      </c>
+      <c r="X8">
+        <v>2</v>
+      </c>
+      <c r="Y8">
+        <v>5</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>235</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>236</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>238</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>148</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>148</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>148</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>148</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>148</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>148</v>
+      </c>
+      <c r="AK8" t="s">
+        <v>148</v>
+      </c>
+      <c r="AL8" t="s">
+        <v>122</v>
+      </c>
+      <c r="AM8" t="s">
+        <v>239</v>
+      </c>
+      <c r="AN8" t="s">
+        <v>240</v>
+      </c>
+      <c r="AO8" t="s">
+        <v>241</v>
+      </c>
+      <c r="AP8" t="s">
+        <v>242</v>
+      </c>
+      <c r="AQ8" t="s">
+        <v>243</v>
+      </c>
+      <c r="AR8" t="s">
+        <v>244</v>
+      </c>
+      <c r="AS8" t="s">
+        <v>245</v>
+      </c>
+      <c r="AT8" t="s">
+        <v>245</v>
+      </c>
+      <c r="AU8" t="s">
+        <v>245</v>
+      </c>
+      <c r="AV8" t="s">
+        <v>246</v>
+      </c>
+      <c r="AW8" t="s">
+        <v>245</v>
+      </c>
+      <c r="AX8" t="s">
+        <v>245</v>
+      </c>
+      <c r="AY8" t="s">
+        <v>247</v>
+      </c>
+      <c r="AZ8" t="s">
+        <v>108</v>
+      </c>
+      <c r="BA8" t="s">
+        <v>108</v>
+      </c>
+      <c r="BB8" t="s">
+        <v>248</v>
+      </c>
+      <c r="BG8" t="s">
+        <v>249</v>
+      </c>
+      <c r="BN8" t="s">
+        <v>250</v>
+      </c>
+      <c r="BP8" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="9" spans="1:68">
+      <c r="A9" t="s">
+        <v>252</v>
+      </c>
+      <c r="B9" t="s">
+        <v>201</v>
+      </c>
+      <c r="C9" t="s">
+        <v>253</v>
+      </c>
+      <c r="D9" t="s">
+        <v>203</v>
+      </c>
+      <c r="E9" t="s">
+        <v>254</v>
+      </c>
+      <c r="F9" t="s">
+        <v>205</v>
+      </c>
+      <c r="G9" t="s">
+        <v>255</v>
+      </c>
+      <c r="H9" t="s">
+        <v>207</v>
+      </c>
+      <c r="I9">
+        <v>5</v>
+      </c>
+      <c r="J9">
+        <v>5</v>
+      </c>
+      <c r="K9">
+        <v>5</v>
+      </c>
+      <c r="L9">
+        <v>5</v>
+      </c>
+      <c r="M9">
+        <v>5</v>
+      </c>
+      <c r="N9">
+        <v>5</v>
+      </c>
+      <c r="O9">
+        <v>4</v>
+      </c>
+      <c r="P9">
+        <v>2</v>
+      </c>
+      <c r="Q9">
+        <v>5</v>
+      </c>
+      <c r="R9">
+        <v>5</v>
+      </c>
+      <c r="S9">
+        <v>3</v>
+      </c>
+      <c r="T9">
+        <v>4</v>
+      </c>
+      <c r="U9">
+        <v>4</v>
+      </c>
+      <c r="V9">
+        <v>4</v>
+      </c>
+      <c r="W9">
+        <v>4</v>
+      </c>
+      <c r="X9">
+        <v>2</v>
+      </c>
+      <c r="Y9">
+        <v>4</v>
+      </c>
+      <c r="Z9">
+        <v>3</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>256</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>257</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>258</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>259</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>148</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>148</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>148</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>148</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>148</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>148</v>
+      </c>
+      <c r="AK9" t="s">
+        <v>148</v>
+      </c>
+      <c r="AL9" t="s">
+        <v>260</v>
+      </c>
+      <c r="AM9" t="s">
+        <v>261</v>
+      </c>
+      <c r="AN9" t="s">
+        <v>262</v>
+      </c>
+      <c r="AO9" t="s">
+        <v>263</v>
+      </c>
+      <c r="AP9" t="s">
+        <v>264</v>
+      </c>
+      <c r="AQ9" t="s">
+        <v>265</v>
+      </c>
+      <c r="AR9" t="s">
+        <v>266</v>
+      </c>
+      <c r="AS9" t="s">
+        <v>266</v>
+      </c>
+      <c r="AT9" t="s">
+        <v>266</v>
+      </c>
+      <c r="AU9" t="s">
+        <v>266</v>
+      </c>
+      <c r="AV9" t="s">
+        <v>266</v>
+      </c>
+      <c r="AW9" t="s">
+        <v>266</v>
+      </c>
+      <c r="AX9" t="s">
+        <v>266</v>
+      </c>
+      <c r="AY9" t="s">
+        <v>266</v>
+      </c>
+      <c r="AZ9" t="s">
+        <v>266</v>
+      </c>
+      <c r="BA9" t="s">
+        <v>266</v>
+      </c>
+      <c r="BB9" t="s">
+        <v>267</v>
+      </c>
+      <c r="BD9" t="s">
+        <v>268</v>
+      </c>
+      <c r="BE9" t="s">
+        <v>269</v>
+      </c>
+      <c r="BF9" t="s">
+        <v>270</v>
+      </c>
+      <c r="BG9" t="s">
+        <v>271</v>
+      </c>
+      <c r="BH9" t="s">
+        <v>272</v>
+      </c>
+      <c r="BI9" t="s">
+        <v>134</v>
+      </c>
+      <c r="BJ9" t="s">
+        <v>134</v>
+      </c>
+      <c r="BK9" t="s">
+        <v>134</v>
+      </c>
+      <c r="BL9" t="s">
+        <v>134</v>
+      </c>
+      <c r="BN9" t="s">
+        <v>273</v>
+      </c>
+      <c r="BO9" t="s">
+        <v>134</v>
+      </c>
+      <c r="BP9" t="s">
+        <v>274</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Code now executes in 0.3 seconds{Enhanced speed by 0.5 secs}
</commit_message>
<xml_diff>
--- a/SummerWork/TEST_OUTPUT.xlsx
+++ b/SummerWork/TEST_OUTPUT.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="313">
   <si>
     <t>School Name :</t>
   </si>
@@ -839,6 +839,120 @@
   </si>
   <si>
     <t>Parents attended trip, using personal vehicles and donating gas costs.  Cooking equipment and gear were provided by parents.  Coordinated with Sunset Bay State Park to do community service for discounted camping rates.  District pays for fuel for busses.</t>
+  </si>
+  <si>
+    <t>Weston</t>
+  </si>
+  <si>
+    <t>Athena-Weston SD 29RJ</t>
+  </si>
+  <si>
+    <t>Ann Vescio</t>
+  </si>
+  <si>
+    <t>Laure Quraesma, Superintendent Athena-Weston Schools</t>
+  </si>
+  <si>
+    <t>ann.vescio@athwest.k12.or.us</t>
+  </si>
+  <si>
+    <t>laure.quaresma@athwest.k12.or.us</t>
+  </si>
+  <si>
+    <t>541-566-3548</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Weston Middle School science department has worked diligently this year to align its science curriculum to the NGSS, to teach through an inquiry model,  and to regularly incorporate STEM activites. The Outdoor School program supported NGSS standards in the areas of PS3 Energy (Cooking Field Study); LS1 From Molecules to Organisms: Structures and Processes (Salmon Life Cycle Field Study and River Invertebrates Inquiry); LS2 Interactions, Energy and Dynamics Relationships in Ecosystems (Fire Impact Field Study, National Weather Service Field Study, Water Quality Field Study, Soil Field Study); LS3 Heredity: Inheritance and Variation of Traits (Salmon Life Cycle Field Study, River Invertebrates Inquiry); ESS2 Weather and Climate (National Weather Service Field Study, Forest Service Field Study); ESS3 Earth and Human Activity (Hike, Forest Service Field Study, Water Quality Field Study, Soil Field Study, River Invertebrates Inquiry); and ETS1 Engineering Design (Cooking Field Study).  Additionally, the water invertibrates, soil, and water quality presentations were inquiry-based lessons. The "campfire cooking" activity was actually a STEM activity which required students to design and then use a "stove" that they built to cook their lunches. These activities were based on the instructional model and on the NGSS curriculum that our students access daily in their science classes. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weston Middle School is a small district located in a very rural area of Umatilla County in eastern Oregon. The school has a free/reduced lunch rate of 59%.  Outdoor School is an opportunity that few of our students would ever have through family resources or through district monies alone. The ability to provide Outdoor School to our students is one way that we can ensure that they have educational opportunities similar to students in wealthier areas of the state. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The field study sessions that we offered in the areas of salmon life cycle, water quality, forest ecosystems/forest fire impact, and soil conservation emphasized the interdendence of urban and rural areas. </t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Observation and Perspective (nature art/nature photography)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Students were required to turn in a completed Field Study Guide after their week of ODS. They debriefed in science classes about their learning at ODS. The two science teachers at Weston Middle School are attending a week-long science training this summer and are part of a science teaching cadre that meets three times annually. Ideas from these trainings will be incorporated into the plan for Outdoor School next school year. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weston Middle School's Outdoor School program included the following partners: National Weather Service, Forest Service, Oregon State Land Laboratory, Department of Environmental Quality, CTUIR (tribe), two community volunteers, 20 parent volunteers, and a retired biology teacher volunteer. </t>
+  </si>
+  <si>
+    <t>N/A--Our ODS program was the last week of May this year. Testing had already been completed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The ODS program required students to assist one another and learn self-sufficiency in the First Aid session, the Water Invertibrates session, the cooking activity, and on the long hike. </t>
+  </si>
+  <si>
+    <t>N/A--Our ODS program was the last week of May this year. There was no time to assess the impact on discipline and classroom management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Students were highly engaged in all facets of Outdoor School. There has been much positive feedback from both students and their parents about the success of the program. In addition, several of the presenters let the school know that the students were very well-behaved, engaged, and respectful. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Several activities promoted problem-solving and strategic thinking. The river invertebrate inquiry project required students to work together to collect invertebrates in a screen while wading in the river. The geocaching and first aid sessions required team work, problem-solving, and strategic thinking as well. Finally, the cooking session was an engineering project where students had to create a working "campfire oven" to cook their lunches. They had to use knowledge of energy and safety to create their ovens. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">We included two Nature Art projects in our ODS program. One was to use items found on a hike to create frames for pictures. The other was to take creative photographs of nature using a variety of perspectives. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The students in our ODS program worked in groups throughout the week. Teachers worked with the teams prior to traveling to the Buck Creek facility to build group work skills through an orientation day. The sessions often required partner or team work to be successful. </t>
+  </si>
+  <si>
+    <t>N/A--Our ODS program was the last week of May this year. There was not time to determine whether or not increased enthusiasm for core subject areas transferred back into the classroom.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The WMS science program has utilized an inquiry approach in the classroom throughout the year. In addition, students have participated in weekly Friday STEM labs all year. The students were able to apply their understanding of these processes in ODS in a variety of sessions including Water Invertebrates, Cooking, Water Quality, and Geocaching/Orienteering. In addition, students frequently utilized scientific vocabulary and background knowledge throughout the ODS program. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The cooking and first aid sessions in particular reinforced the application of scientific and civic processes in real-world situations. Students had to design a functional campfire "oven" with limited supplies in order to cook their stew for lunch. In the first aid sessions, students were given scenarios in which to apply their knowledge of first aid and rescue. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Students kept notes in their ODS Field Study Guides as part of the program. They recorded notes and observations from all of their sessions following Notebooking protocols that they have utilized all year in their science and Friday STEM classes. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Students applied their knowledge of geography concepts in the Geocaching/Orienteering session which was run by their geography teacher. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">All 6th graders but one who was on a family trip attended ODS. This included special education students as well as students of all abilities and learning styles. Support personnel attended to ensure that all programming was accessible to our special education students. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Students in the Athena-Weston School District come from a very rural area of Umatilla County. All students but one who was on a family trip attended ODS. The daytime-only format was important to our participation rate as we have a number of students and/or parents who indicated that they were uncomfortable with an overnight scenario. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">All 6th grade students but one who was on a family trip attended ODS. This included our special education students. We sent adult support to ensure full participation from two autistic students and one Down's Syndrome student. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">We had a student with Down's Syndrome participate in ODS. He has some physical limitations. Therefore we sent adult support to ensure that the program was accessible. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weston Middle School's free and reduced lunch rate is 59%. We provided string packs, water bottles, binoculars, notebooks and writing utensils, t-shirts, reimbursable school lunches, water, and snacks at no charge to students to ensure that ODS was not a financial burden to any families. </t>
+  </si>
+  <si>
+    <t>21% of our 6th grade students identify as American Indian/Alaska Native. We included a presentation provided by the CTUIR tribal offices in our ODS program.</t>
+  </si>
+  <si>
+    <t>1% of our 6th grade students identify as Asian.</t>
+  </si>
+  <si>
+    <t>1% of our 6th grade students identify as African American.</t>
+  </si>
+  <si>
+    <t>11% of our 6th grade students identify as Hispanic/Latino.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transporting students to ODS daily during school hours versus an overnight program ensured that all 6th graders attended ODS. We will continue this format next year. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This was our first ODS program. Therefore we had no existing equipment for ODS. We purchased high quality radios so that the adult leaders could communicate as there was no reliable cell phone service in the Buck Creek area. This purchase would not have been feasible through our building budget. </t>
+  </si>
+  <si>
+    <t>Weston Middle School accessed local resources for its field study sessions. Those partners included the National Weather Service, CTUIR (tribal), OSU Land Lab scientists, DEQ Water Quality offices, and the Forest Service. In addition, a local retired biology teacher conducted a field study session. More than 20 parents volunteered throughout the week to chaperone, and four Weston Middle School teachers conducted field studies for ODS. We used the IMESD-owned Buck Creek facility at no charge for the ODS site.</t>
   </si>
 </sst>
 </file>
@@ -1187,7 +1301,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BP9"/>
+  <dimension ref="A1:BP10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2747,6 +2861,209 @@
         <v>274</v>
       </c>
     </row>
+    <row r="10" spans="1:68">
+      <c r="A10" t="s">
+        <v>275</v>
+      </c>
+      <c r="B10" t="s">
+        <v>276</v>
+      </c>
+      <c r="C10" t="s">
+        <v>277</v>
+      </c>
+      <c r="D10" t="s">
+        <v>278</v>
+      </c>
+      <c r="E10" t="s">
+        <v>279</v>
+      </c>
+      <c r="F10" t="s">
+        <v>280</v>
+      </c>
+      <c r="G10" t="s">
+        <v>281</v>
+      </c>
+      <c r="I10">
+        <v>5</v>
+      </c>
+      <c r="J10">
+        <v>2</v>
+      </c>
+      <c r="K10">
+        <v>2</v>
+      </c>
+      <c r="L10">
+        <v>4</v>
+      </c>
+      <c r="M10">
+        <v>3</v>
+      </c>
+      <c r="N10">
+        <v>5</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <v>3</v>
+      </c>
+      <c r="Q10">
+        <v>3</v>
+      </c>
+      <c r="R10">
+        <v>4</v>
+      </c>
+      <c r="S10">
+        <v>2</v>
+      </c>
+      <c r="T10">
+        <v>1</v>
+      </c>
+      <c r="U10">
+        <v>1</v>
+      </c>
+      <c r="V10">
+        <v>2</v>
+      </c>
+      <c r="W10">
+        <v>5</v>
+      </c>
+      <c r="X10">
+        <v>2</v>
+      </c>
+      <c r="Y10">
+        <v>2</v>
+      </c>
+      <c r="Z10">
+        <v>2</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>282</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>134</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>283</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>284</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>285</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AI10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL10" t="s">
+        <v>286</v>
+      </c>
+      <c r="AM10" t="s">
+        <v>287</v>
+      </c>
+      <c r="AN10" t="s">
+        <v>288</v>
+      </c>
+      <c r="AO10" t="s">
+        <v>289</v>
+      </c>
+      <c r="AP10" t="s">
+        <v>290</v>
+      </c>
+      <c r="AQ10" t="s">
+        <v>291</v>
+      </c>
+      <c r="AR10" t="s">
+        <v>292</v>
+      </c>
+      <c r="AS10" t="s">
+        <v>293</v>
+      </c>
+      <c r="AT10" t="s">
+        <v>294</v>
+      </c>
+      <c r="AU10" t="s">
+        <v>295</v>
+      </c>
+      <c r="AV10" t="s">
+        <v>296</v>
+      </c>
+      <c r="AW10" t="s">
+        <v>297</v>
+      </c>
+      <c r="AX10" t="s">
+        <v>298</v>
+      </c>
+      <c r="AY10" t="s">
+        <v>134</v>
+      </c>
+      <c r="AZ10" t="s">
+        <v>299</v>
+      </c>
+      <c r="BA10" t="s">
+        <v>300</v>
+      </c>
+      <c r="BB10" t="s">
+        <v>301</v>
+      </c>
+      <c r="BC10" t="s">
+        <v>302</v>
+      </c>
+      <c r="BD10" t="s">
+        <v>134</v>
+      </c>
+      <c r="BE10" t="s">
+        <v>303</v>
+      </c>
+      <c r="BF10" t="s">
+        <v>304</v>
+      </c>
+      <c r="BG10" t="s">
+        <v>305</v>
+      </c>
+      <c r="BH10" t="s">
+        <v>306</v>
+      </c>
+      <c r="BI10" t="s">
+        <v>307</v>
+      </c>
+      <c r="BJ10" t="s">
+        <v>134</v>
+      </c>
+      <c r="BK10" t="s">
+        <v>308</v>
+      </c>
+      <c r="BL10" t="s">
+        <v>309</v>
+      </c>
+      <c r="BM10" t="s">
+        <v>134</v>
+      </c>
+      <c r="BN10" t="s">
+        <v>310</v>
+      </c>
+      <c r="BO10" t="s">
+        <v>311</v>
+      </c>
+      <c r="BP10" t="s">
+        <v>312</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>